<commit_message>
Analisis electrico, no me ha dado a mucho mas luego sigo si veis este coment
</commit_message>
<xml_diff>
--- a/04 - Análisis consumo/AnalisisConsumo.xlsx
+++ b/04 - Análisis consumo/AnalisisConsumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuvaes-my.sharepoint.com/personal/rubenfrancisco_serrano_alumnos_uva_es/Documents/Teleco/Master/Primer cuatrimestre/TP/SE/04 - Análisis consumo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_AD4D2F04E46CFB4ACB3E20F29557D0D8683EDF1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B5E346-8786-4347-BA2A-6510212312DA}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_AD4D2F04E46CFB4ACB3E20F29557D0D8683EDF1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{899A7FB2-5B9D-48EA-AB28-6373135CB052}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Análisis eléctrico</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FPGA ICE</t>
+  </si>
+  <si>
+    <t>Memoria NORFlash 32Mb</t>
+  </si>
+  <si>
+    <t>Board 1</t>
   </si>
 </sst>
 </file>
@@ -135,14 +144,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,94 +451,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -540,62 +549,62 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -606,122 +615,164 @@
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -729,7 +780,7 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Añadidos componentes de la PCB1 al análisis eléctrico y térmico. Hay componentes de los cuales no encuentro información
</commit_message>
<xml_diff>
--- a/04 - Análisis consumo/AnalisisConsumo.xlsx
+++ b/04 - Análisis consumo/AnalisisConsumo.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarmartincasares/Desktop/Ing. Telecomunicaciones/Master/1er Cuatrimestre/TALLER PROYECTOS/SE/TP1SE/04 - Análisis consumo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA588D-DD5A-1E40-BB1F-D12D97D4F74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB3D4B0-6857-48FF-A1D5-70887D757FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23895" yWindow="4350" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumo de energía PCB0" sheetId="1" r:id="rId1"/>
-    <sheet name="Disipación de potencia" sheetId="2" r:id="rId2"/>
+    <sheet name="Consumo de energía PCB1" sheetId="3" r:id="rId2"/>
+    <sheet name="Disipación de potencia" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
   <si>
     <t>Componentes a 5V</t>
   </si>
@@ -139,6 +140,39 @@
   </si>
   <si>
     <t>230ºC/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memoria NOR Flash 32 Mbit IS25LP032D-JNLE </t>
+  </si>
+  <si>
+    <t>12 (Active Read Current)</t>
+  </si>
+  <si>
+    <t>Componentes a 1V2</t>
+  </si>
+  <si>
+    <t>Página 99. Datasheet</t>
+  </si>
+  <si>
+    <t>FPGA ICE40HX4K-TQ144</t>
+  </si>
+  <si>
+    <t>Diodo 1N4448HWS</t>
+  </si>
+  <si>
+    <t>Resistencia térmica (ºC/W)</t>
+  </si>
+  <si>
+    <t>Temperatura (ºC)</t>
+  </si>
+  <si>
+    <t>-65 a 150</t>
+  </si>
+  <si>
+    <t>Página 1. Datasheet</t>
+  </si>
+  <si>
+    <t>-40 a 125</t>
   </si>
 </sst>
 </file>
@@ -186,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,6 +232,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,19 +523,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1"/>
-    <col min="2" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -503,14 +544,14 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -519,7 +560,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,7 +577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -553,35 +594,35 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -590,7 +631,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,7 +648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -624,7 +665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -633,7 +674,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -647,14 +688,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -663,7 +704,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -680,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -697,7 +738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -714,56 +755,56 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -772,14 +813,14 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -796,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -813,7 +854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -830,7 +871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -839,7 +880,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -856,7 +897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -873,7 +914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -890,21 +931,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -924,12 +965,330 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DDC9D9-1F46-47B6-93CC-87CC0629DA96}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1">
+        <v>200</v>
+      </c>
+      <c r="C25" s="1">
+        <v>625</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C26" s="1">
+        <v>163</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A15:E15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD9430D-8F46-4B9F-A350-3791495ED648}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>